<commit_message>
changes for dialog showing
</commit_message>
<xml_diff>
--- a/files/export.XLSX
+++ b/files/export.XLSX
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mseidler\workspace_luna\PromptToBoatConverter\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1345,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="G58" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,13 +2123,13 @@
         <v>42586</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I16" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="J16" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="K16">
         <v>70</v>
@@ -4477,13 +4473,13 @@
         <v>42583</v>
       </c>
       <c r="H63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I63" s="2">
         <v>0.5</v>
       </c>
       <c r="J63" s="2">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="K63">
         <v>100</v>

</xml_diff>